<commit_message>
adapt two advices from teacher in my paper
</commit_message>
<xml_diff>
--- a/Mypaper/tables/4.7二级风险因素概率样本统计分析.xlsx
+++ b/Mypaper/tables/4.7二级风险因素概率样本统计分析.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24225" windowHeight="12540"/>
+    <workbookView windowWidth="14910" windowHeight="13200"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -556,13 +556,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="0.000_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="176" formatCode="0.000_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -571,13 +571,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10.5"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -589,34 +582,6 @@
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -627,6 +592,57 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="宋体"/>
@@ -634,8 +650,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -649,25 +690,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -681,55 +721,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -767,19 +760,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -791,163 +904,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -976,6 +969,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -994,8 +1005,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1022,24 +1033,6 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1078,168 +1071,165 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1593,7 +1583,7 @@
   <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A1" sqref="A1:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
@@ -1611,186 +1601,186 @@
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>0.868</v>
       </c>
     </row>
     <row r="3" ht="15" spans="1:2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>0.75</v>
       </c>
     </row>
     <row r="4" ht="15" spans="1:2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>0.8</v>
       </c>
     </row>
     <row r="5" ht="15" spans="1:2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>0.352</v>
       </c>
     </row>
     <row r="6" ht="15" spans="1:2">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>0.391</v>
       </c>
     </row>
     <row r="7" ht="15" spans="1:2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>0.263</v>
       </c>
     </row>
     <row r="8" ht="15" spans="1:2">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>0.274</v>
       </c>
     </row>
     <row r="9" ht="15" spans="1:2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>0.8</v>
       </c>
     </row>
     <row r="10" ht="15" spans="1:2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>0.548</v>
       </c>
     </row>
     <row r="11" ht="15" spans="1:2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>0.586</v>
       </c>
     </row>
     <row r="12" ht="15" spans="1:2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>0.636</v>
       </c>
     </row>
     <row r="13" ht="15" spans="1:2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>0.881</v>
       </c>
     </row>
     <row r="14" ht="15" spans="1:2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <v>0.55</v>
       </c>
     </row>
     <row r="15" ht="15" spans="1:2">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>0.807</v>
       </c>
     </row>
     <row r="16" ht="15" spans="1:2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>0.506</v>
       </c>
     </row>
     <row r="17" ht="15" spans="1:2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>0.332</v>
       </c>
     </row>
     <row r="18" ht="15" spans="1:2">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>0.318</v>
       </c>
     </row>
     <row r="19" ht="15" spans="1:2">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>0.324</v>
       </c>
     </row>
     <row r="20" ht="15" spans="1:2">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>0.469</v>
       </c>
     </row>
     <row r="21" ht="15" spans="1:2">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>0.344</v>
       </c>
     </row>
     <row r="22" ht="15" spans="1:2">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>0.273</v>
       </c>
     </row>
     <row r="23" ht="15" spans="1:2">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>0.125</v>
       </c>
     </row>
     <row r="24" ht="15" spans="1:2">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="1">
         <v>0.168</v>
       </c>
     </row>

</xml_diff>